<commit_message>
begin testing with bad data
</commit_message>
<xml_diff>
--- a/parameters/Sensor_Parameters.xlsx
+++ b/parameters/Sensor_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgrant/Library/CloudStorage/OneDrive-Personal/GitHub/geocoug/ASV-CTD-Processing/parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54d68f46f5829c2c/GitHub/geocoug/asv-ctd-qa/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989F909C-1B5D-244D-96CB-C046CB0729CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{989F909C-1B5D-244D-96CB-C046CB0729CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FD093F0-E3E3-2844-8C83-5BCBC3A99D1B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="17280" windowHeight="21580" tabRatio="822" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" tabRatio="822" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -809,12 +809,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -822,7 +821,7 @@
     <col min="1" max="1" width="14.83203125" customWidth="1"/>
     <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="51.5" style="8" customWidth="1"/>
+    <col min="4" max="4" width="117.33203125" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18.5" customWidth="1"/>
     <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="21.1640625" customWidth="1"/>
@@ -862,7 +861,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>74</v>
       </c>
@@ -891,7 +890,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
@@ -920,7 +919,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>74</v>
       </c>
@@ -949,7 +948,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>74</v>
       </c>
@@ -978,7 +977,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
@@ -1007,7 +1006,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>74</v>
       </c>
@@ -1164,7 +1163,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>103</v>
       </c>
@@ -1196,7 +1195,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>103</v>
       </c>
@@ -1228,7 +1227,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>103</v>
       </c>
@@ -1260,7 +1259,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>103</v>
       </c>
@@ -1292,7 +1291,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>103</v>
       </c>
@@ -1324,7 +1323,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>103</v>
       </c>
@@ -1356,7 +1355,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>103</v>
       </c>
@@ -1388,7 +1387,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>103</v>
       </c>
@@ -1548,7 +1547,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>104</v>
       </c>
@@ -1580,7 +1579,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>104</v>
       </c>
@@ -1612,7 +1611,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>104</v>
       </c>
@@ -1644,7 +1643,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>104</v>
       </c>
@@ -1676,7 +1675,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>104</v>
       </c>
@@ -1708,7 +1707,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>104</v>
       </c>
@@ -1740,7 +1739,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>104</v>
       </c>
@@ -1772,7 +1771,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>104</v>
       </c>
@@ -1932,7 +1931,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>105</v>
       </c>
@@ -1964,7 +1963,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>105</v>
       </c>
@@ -1996,7 +1995,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>105</v>
       </c>
@@ -2028,7 +2027,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="39" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>105</v>
       </c>
@@ -2060,7 +2059,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>105</v>
       </c>
@@ -2092,7 +2091,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>105</v>
       </c>
@@ -2124,7 +2123,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>105</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>105</v>
       </c>
@@ -2316,7 +2315,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>106</v>
       </c>
@@ -2348,7 +2347,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>106</v>
       </c>
@@ -2380,7 +2379,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>106</v>
       </c>
@@ -2412,7 +2411,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="51" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>106</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>106</v>
       </c>
@@ -2476,7 +2475,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>106</v>
       </c>
@@ -2508,7 +2507,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="54" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
@@ -2540,7 +2539,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="55" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>106</v>
       </c>
@@ -2700,7 +2699,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>107</v>
       </c>
@@ -2732,7 +2731,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>107</v>
       </c>
@@ -2764,7 +2763,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>107</v>
       </c>
@@ -2796,7 +2795,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>107</v>
       </c>
@@ -2828,7 +2827,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>107</v>
       </c>
@@ -2860,7 +2859,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>107</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>107</v>
       </c>
@@ -2924,7 +2923,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>107</v>
       </c>
@@ -3084,7 +3083,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>108</v>
       </c>
@@ -3116,7 +3115,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>108</v>
       </c>
@@ -3148,7 +3147,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>108</v>
       </c>
@@ -3180,7 +3179,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="75" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>108</v>
       </c>
@@ -3212,7 +3211,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>108</v>
       </c>
@@ -3244,7 +3243,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>108</v>
       </c>
@@ -3276,7 +3275,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>108</v>
       </c>
@@ -3308,7 +3307,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>108</v>
       </c>
@@ -3468,7 +3467,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>109</v>
       </c>
@@ -3500,7 +3499,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>109</v>
       </c>
@@ -3532,7 +3531,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>109</v>
       </c>
@@ -3564,7 +3563,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>109</v>
       </c>
@@ -3596,7 +3595,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>109</v>
       </c>
@@ -3628,7 +3627,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>109</v>
       </c>
@@ -3660,7 +3659,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>109</v>
       </c>
@@ -3692,7 +3691,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>109</v>
       </c>
@@ -3852,7 +3851,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>110</v>
       </c>
@@ -3884,7 +3883,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>110</v>
       </c>
@@ -3916,7 +3915,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>110</v>
       </c>
@@ -3948,7 +3947,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>110</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>110</v>
       </c>
@@ -4012,7 +4011,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>110</v>
       </c>
@@ -4044,7 +4043,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>110</v>
       </c>
@@ -4076,7 +4075,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>110</v>
       </c>
@@ -4224,7 +4223,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>111</v>
       </c>
@@ -4253,7 +4252,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>111</v>
       </c>
@@ -4282,7 +4281,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>111</v>
       </c>
@@ -4311,7 +4310,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>111</v>
       </c>
@@ -4340,7 +4339,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>111</v>
       </c>
@@ -4369,7 +4368,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
@@ -4398,7 +4397,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>111</v>
       </c>
@@ -4427,7 +4426,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>111</v>
       </c>
@@ -4572,7 +4571,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>112</v>
       </c>
@@ -4601,7 +4600,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>112</v>
       </c>
@@ -4630,7 +4629,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>112</v>
       </c>
@@ -4659,7 +4658,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>112</v>
       </c>
@@ -4688,7 +4687,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>112</v>
       </c>
@@ -4717,7 +4716,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>112</v>
       </c>
@@ -4746,7 +4745,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>112</v>
       </c>
@@ -4775,7 +4774,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>112</v>
       </c>
@@ -4804,7 +4803,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>112</v>
       </c>
@@ -4838,16 +4837,7 @@
       <c r="B129" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J128" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="climate_max"/>
-        <filter val="climate_min"/>
-        <filter val="sensor_max"/>
-        <filter val="sensor_min"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J128" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
update readme, unix epoch for datetime calcs, rm ioos_qc from requirements.txt
</commit_message>
<xml_diff>
--- a/parameters/Sensor_Parameters.xlsx
+++ b/parameters/Sensor_Parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54d68f46f5829c2c/GitHub/geocoug/asv-ctd-qa/parameters/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54d68f46f5829c2c/GitHub/integral/asv-ctd-qa/parameters/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="13_ncr:1_{989F909C-1B5D-244D-96CB-C046CB0729CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1FD093F0-E3E3-2844-8C83-5BCBC3A99D1B}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="13_ncr:1_{989F909C-1B5D-244D-96CB-C046CB0729CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32E792DD-D43C-6C43-8BAA-4CA524998579}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" tabRatio="822" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20160" tabRatio="822" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="5" r:id="rId1"/>
@@ -812,8 +812,8 @@
   <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>